<commit_message>
Adicionados novos tratamentos de exceções
</commit_message>
<xml_diff>
--- a/agendamentos.xlsx
+++ b/agendamentos.xlsx
@@ -390,10 +390,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -423,6 +423,28 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>21/02/2024</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>5533991965662</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>